<commit_message>
Print last Guide sequence
Print last Guide sequence
</commit_message>
<xml_diff>
--- a/data/evaluation.xlsx
+++ b/data/evaluation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahdiye\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahdiye\IdeaProjects\comp680\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Guide Sequence</t>
   </si>
@@ -69,13 +69,70 @@
   </si>
   <si>
     <t>TCCTGACAATCGATAGGTACCTG</t>
+  </si>
+  <si>
+    <t>Frock_EMX</t>
+  </si>
+  <si>
+    <t>GAGTCCGAGCAGAAGAAGAAGGG</t>
+  </si>
+  <si>
+    <t>Frock_RAG1A</t>
+  </si>
+  <si>
+    <t>GCCTCTTTCCCACCCACCTTGGG</t>
+  </si>
+  <si>
+    <t>GTGGCGCATTGCCACGAAGCAGG</t>
+  </si>
+  <si>
+    <t>CCAGCGACGTGCCCCAGGACGGG</t>
+  </si>
+  <si>
+    <t>TGCGGAGGGGAGTGGACTTAGGG</t>
+  </si>
+  <si>
+    <t>CGTGGGCCCAAGCTGGACTCTGG</t>
+  </si>
+  <si>
+    <t>CACATATTAAATTTTCAGAATGG</t>
+  </si>
+  <si>
+    <t>TCAGGCAAGGATCAGCAGCAAGG</t>
+  </si>
+  <si>
+    <t>CTCAGATGCCTCAAAGTCATGGG</t>
+  </si>
+  <si>
+    <t>CTTGTTCCTGCTGGCTCTGAGGG</t>
+  </si>
+  <si>
+    <t>Wang_WAS-CR5</t>
+  </si>
+  <si>
+    <t>CCCTGTGTCTCTGGATGGATGGG</t>
+  </si>
+  <si>
+    <t>ACTAGTGAATGAAACTGCAGAGG</t>
+  </si>
+  <si>
+    <t>TTTGTGCTTATCTTAATACCAGG</t>
+  </si>
+  <si>
+    <t>AACCCCCCCAGGTTACCTGTGGG</t>
+  </si>
+  <si>
+    <t>CGGGTGGATCACCTGAGGTCAGG</t>
+  </si>
+  <si>
+    <t>more than least similarity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +140,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,8 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,8 +572,11 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,7 +619,152 @@
         <v>-0.46574163307160998</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>-0.32079273748575998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>-0.32079273748575998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>-0.30839006191383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>-0.33592883798290502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>-0.40116985011574902</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>-0.40331181544619299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>-0.403228086189868</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>-0.38898218306267601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39">
+        <v>-0.38215702939849999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40">
+        <v>-0.37908082937397403</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41">
+        <v>-0.36456938458516402</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42">
+        <v>-0.35465526773894401</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>